<commit_message>
Approach 1 Final (without experience factor)
</commit_message>
<xml_diff>
--- a/results/jdk_1_resume_score.xlsx
+++ b/results/jdk_1_resume_score.xlsx
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9232060979362313</v>
+        <v>2.367275367578336</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.616030489681156</v>
+        <v>3.983303952131626</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3.186643161705301</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>2.315550409313988</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1.552801859005456</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.7980774557353087</v>
       </c>
     </row>
     <row r="3">
@@ -584,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>2.76229894385294</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>3.859250682189979</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>3.186478240571118</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>1.588926508372374</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>2.414540344278287</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>

</xml_diff>

<commit_message>
prompt change and experience integration
</commit_message>
<xml_diff>
--- a/results/jdk_1_resume_score.xlsx
+++ b/results/jdk_1_resume_score.xlsx
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.367275367578336</v>
+        <v>3.601030655423489</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -508,23 +508,23 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>6.373286323410602</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Literature Society IITJ Website</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>3.983303952131626</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Literature Society IITJ Website</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>3.186643161705301</v>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>CloudPhysician's Vital Extraction Challenge</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2.315550409313988</v>
+        <v>0</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>1.552801859005456</v>
+        <v>2.717403253259548</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.7980774557353087</v>
+        <v>1.330129092892181</v>
       </c>
     </row>
     <row r="3">
@@ -548,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2.550588267952786</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2.711194164626598</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>2.389982371278975</v>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -584,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.76229894385294</v>
+        <v>4.282329885966153</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3.859250682189979</v>
+        <v>6.174801091503967</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3.186478240571118</v>
+        <v>2.389858680428339</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1.588926508372374</v>
+        <v>0</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>2.414540344278287</v>
+        <v>0</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>

</xml_diff>